<commit_message>
got denver and seattle weather
</commit_message>
<xml_diff>
--- a/Seattle_weather.xlsx
+++ b/Seattle_weather.xlsx
@@ -468,7 +468,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Percipitation_mm</t>
+          <t>Precipitation_mm</t>
         </is>
       </c>
     </row>
@@ -487,7 +487,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -509,7 +509,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -531,7 +531,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -553,7 +553,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -575,7 +575,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -597,7 +597,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -619,7 +619,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -641,7 +641,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -663,7 +663,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -685,7 +685,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -707,7 +707,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -729,7 +729,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -751,7 +751,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -773,7 +773,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -795,7 +795,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -817,7 +817,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -839,7 +839,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -861,7 +861,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -883,7 +883,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -905,7 +905,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -927,7 +927,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -949,7 +949,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -971,7 +971,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -993,7 +993,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1015,7 +1015,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1037,7 +1037,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1081,7 +1081,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -1125,7 +1125,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1147,7 +1147,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -1235,7 +1235,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -1279,7 +1279,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -1323,7 +1323,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -1345,7 +1345,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -1367,7 +1367,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -1389,7 +1389,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -1433,7 +1433,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -1455,7 +1455,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -1477,7 +1477,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -1499,7 +1499,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>spring</t>
+          <t>summer</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -1575,412 +1575,500 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Percipitation_mm</t>
+          <t>Precipitation_mm</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44541</v>
+        <v>44498</v>
       </c>
       <c r="B2" t="n">
-        <v>5.7</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="E2" t="inlineStr"/>
+        <v>0.4</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F2" t="n">
-        <v>0.4064</v>
+        <v>1.905</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44541.04166666666</v>
+        <v>44498.04166666666</v>
       </c>
       <c r="B3" t="n">
-        <v>5.800000000000001</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="E3" t="inlineStr"/>
+        <v>0.4</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F3" t="n">
-        <v>0.9906</v>
+        <v>0.801076923076923</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44541.08333333334</v>
+        <v>44498.08333333334</v>
       </c>
       <c r="B4" t="n">
-        <v>5.9</v>
+        <v>9</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="E4" t="inlineStr"/>
+        <v>0.5</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F4" t="n">
-        <v>1.016</v>
+        <v>1.733176470588235</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44541.125</v>
+        <v>44498.125</v>
       </c>
       <c r="B5" t="n">
-        <v>6</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="E5" t="inlineStr"/>
+        <v>0.5</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F5" t="n">
-        <v>0.508</v>
+        <v>1.23825</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44541.16666666666</v>
+        <v>44498.16666666666</v>
       </c>
       <c r="B6" t="n">
-        <v>6.2</v>
+        <v>8.5</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
+        <v>0.4</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F6" t="n">
-        <v>0.4103076923076923</v>
+        <v>1.172307692307692</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44541.20833333334</v>
+        <v>44498.20833333334</v>
       </c>
       <c r="B7" t="n">
-        <v>6.4</v>
+        <v>8.4</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
+        <v>0.5</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F7" t="n">
-        <v>0.4233333333333333</v>
+        <v>0.7281333333333334</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44541.25</v>
+        <v>44498.25</v>
       </c>
       <c r="B8" t="n">
-        <v>6.300000000000001</v>
+        <v>8.4</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="E8" t="inlineStr"/>
+        <v>0.5</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F8" t="n">
-        <v>0.2328333333333333</v>
+        <v>0.7619999999999999</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44541.29166666666</v>
+        <v>44498.29166666666</v>
       </c>
       <c r="B9" t="n">
-        <v>6</v>
+        <v>8.1</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="E9" t="inlineStr"/>
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F9" t="n">
-        <v>0.4717142857142857</v>
+        <v>0.4535714285714286</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44541.33333333334</v>
+        <v>44498.33333333334</v>
       </c>
       <c r="B10" t="n">
-        <v>5.800000000000001</v>
+        <v>7.800000000000001</v>
       </c>
       <c r="C10" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" t="inlineStr"/>
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F10" t="n">
-        <v>0.3064666666666667</v>
+        <v>0.3321538461538461</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44541.375</v>
+        <v>44498.375</v>
       </c>
       <c r="B11" t="n">
-        <v>6.2</v>
+        <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="D11" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="E11" t="inlineStr"/>
+        <v>0.4</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F11" t="n">
-        <v>0.1582307692307692</v>
+        <v>0.1953846153846154</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44541.41666666666</v>
+        <v>44498.41666666666</v>
       </c>
       <c r="B12" t="n">
-        <v>6.600000000000001</v>
+        <v>10.5</v>
       </c>
       <c r="C12" t="n">
-        <v>136</v>
+        <v>39</v>
       </c>
       <c r="D12" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="E12" t="inlineStr"/>
+        <v>0.5</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F12" t="n">
-        <v>0.4318</v>
+        <v>0.1693333333333333</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>44541.45833333334</v>
+        <v>44498.45833333334</v>
       </c>
       <c r="B13" t="n">
-        <v>7</v>
+        <v>11.2</v>
       </c>
       <c r="C13" t="n">
-        <v>199</v>
+        <v>64</v>
       </c>
       <c r="D13" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="E13" t="inlineStr"/>
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F13" t="n">
-        <v>0.4064</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44541.5</v>
+        <v>44498.5</v>
       </c>
       <c r="B14" t="n">
-        <v>7.2</v>
+        <v>12</v>
       </c>
       <c r="C14" t="n">
-        <v>185</v>
+        <v>122</v>
       </c>
       <c r="D14" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="E14" t="inlineStr"/>
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F14" t="n">
-        <v>0.004166666666666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>44541.54166666666</v>
+        <v>44498.54166666666</v>
       </c>
       <c r="B15" t="n">
-        <v>7.100000000000001</v>
+        <v>12.2</v>
       </c>
       <c r="C15" t="n">
-        <v>170</v>
+        <v>50</v>
       </c>
       <c r="D15" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="E15" t="inlineStr"/>
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>0.001923076923076923</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>44541.58333333334</v>
+        <v>44498.58333333334</v>
       </c>
       <c r="B16" t="n">
-        <v>6.800000000000001</v>
+        <v>12</v>
       </c>
       <c r="C16" t="n">
-        <v>126</v>
+        <v>45</v>
       </c>
       <c r="D16" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="E16" t="inlineStr"/>
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F16" t="n">
-        <v>0.1549</v>
+        <v>0.003571428571428572</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>44541.625</v>
+        <v>44498.625</v>
       </c>
       <c r="B17" t="n">
-        <v>6.4</v>
+        <v>11.8</v>
       </c>
       <c r="C17" t="n">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="D17" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="E17" t="inlineStr"/>
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F17" t="n">
-        <v>0.4493846153846154</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>44541.66666666666</v>
+        <v>44498.66666666666</v>
       </c>
       <c r="B18" t="n">
-        <v>5.7</v>
+        <v>11</v>
       </c>
       <c r="C18" t="n">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D18" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="E18" t="inlineStr"/>
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F18" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>44541.70833333334</v>
+        <v>44498.70833333334</v>
       </c>
       <c r="B19" t="n">
-        <v>5.300000000000001</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="D19" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="E19" t="inlineStr"/>
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F19" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>44541.75</v>
+        <v>44498.75</v>
       </c>
       <c r="B20" t="n">
-        <v>4.800000000000001</v>
+        <v>6.7</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
-      </c>
-      <c r="E20" t="inlineStr"/>
+        <v>0.8</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>44541.79166666666</v>
+        <v>44498.79166666666</v>
       </c>
       <c r="B21" t="n">
-        <v>4.4</v>
+        <v>6.100000000000001</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E21" t="inlineStr"/>
+        <v>0.9</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>44541.83333333334</v>
+        <v>44498.83333333334</v>
       </c>
       <c r="B22" t="n">
-        <v>4.100000000000001</v>
+        <v>5.5</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
-      </c>
-      <c r="E22" t="inlineStr"/>
+        <v>0.9</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F22" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>44541.875</v>
+        <v>44498.875</v>
       </c>
       <c r="B23" t="n">
-        <v>4</v>
+        <v>4.9</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="E23" t="inlineStr"/>
+        <v>0.9</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F23" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>44541.91666666666</v>
+        <v>44498.91666666666</v>
       </c>
       <c r="B24" t="n">
-        <v>3.7</v>
+        <v>4.600000000000001</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
@@ -1988,122 +2076,150 @@
       <c r="D24" t="n">
         <v>1</v>
       </c>
-      <c r="E24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F24" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>44541.95833333334</v>
+        <v>44498.95833333334</v>
       </c>
       <c r="B25" t="n">
-        <v>3.6</v>
+        <v>4.3</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="E25" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F25" t="n">
-        <v>0.01953846153846154</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>44542</v>
+        <v>44499</v>
       </c>
       <c r="B26" t="n">
-        <v>3.5</v>
+        <v>3.9</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
-      </c>
-      <c r="E26" t="inlineStr"/>
+        <v>0.9</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F26" t="n">
-        <v>0.889</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>44542.04166666666</v>
+        <v>44499.04166666666</v>
       </c>
       <c r="B27" t="n">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
-      </c>
-      <c r="E27" t="inlineStr"/>
+        <v>0.8</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F27" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>44542.08333333334</v>
+        <v>44499.08333333334</v>
       </c>
       <c r="B28" t="n">
-        <v>3.6</v>
+        <v>3.9</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="E28" t="inlineStr"/>
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F28" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>44542.125</v>
+        <v>44499.125</v>
       </c>
       <c r="B29" t="n">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="E29" t="inlineStr"/>
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F29" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>44542.16666666666</v>
+        <v>44499.16666666666</v>
       </c>
       <c r="B30" t="n">
-        <v>3.1</v>
+        <v>3.7</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="E30" t="inlineStr"/>
+        <v>0.8</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F30" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>44542.20833333334</v>
+        <v>44499.20833333334</v>
       </c>
       <c r="B31" t="n">
         <v>2.9</v>
@@ -2112,235 +2228,287 @@
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="E31" t="inlineStr"/>
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F31" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>44542.25</v>
+        <v>44499.25</v>
       </c>
       <c r="B32" t="n">
-        <v>2.9</v>
+        <v>2.7</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="E32" t="inlineStr"/>
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F32" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>44542.29166666666</v>
+        <v>44499.29166666666</v>
       </c>
       <c r="B33" t="n">
-        <v>2.9</v>
+        <v>2.2</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="E33" t="inlineStr"/>
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F33" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>44542.33333333334</v>
+        <v>44499.33333333334</v>
       </c>
       <c r="B34" t="n">
-        <v>3</v>
+        <v>2.4</v>
       </c>
       <c r="C34" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D34" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="E34" t="inlineStr"/>
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F34" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>44542.375</v>
+        <v>44499.375</v>
       </c>
       <c r="B35" t="n">
-        <v>3.3</v>
+        <v>4.5</v>
       </c>
       <c r="C35" t="n">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="D35" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="E35" t="inlineStr"/>
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F35" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>44542.41666666666</v>
+        <v>44499.41666666666</v>
       </c>
       <c r="B36" t="n">
-        <v>3.5</v>
+        <v>6.600000000000001</v>
       </c>
       <c r="C36" t="n">
-        <v>144</v>
+        <v>289</v>
       </c>
       <c r="D36" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="E36" t="inlineStr"/>
+        <v>0.8</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F36" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>44542.45833333334</v>
+        <v>44499.45833333334</v>
       </c>
       <c r="B37" t="n">
-        <v>3.6</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="C37" t="n">
-        <v>215</v>
+        <v>407</v>
       </c>
       <c r="D37" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="E37" t="inlineStr"/>
+        <v>0.9</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F37" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>44542.5</v>
+        <v>44499.5</v>
       </c>
       <c r="B38" t="n">
-        <v>4</v>
+        <v>10.6</v>
       </c>
       <c r="C38" t="n">
-        <v>135</v>
+        <v>476</v>
       </c>
       <c r="D38" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="E38" t="inlineStr"/>
+        <v>0.9</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F38" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>44542.54166666666</v>
+        <v>44499.54166666666</v>
       </c>
       <c r="B39" t="n">
-        <v>4.3</v>
+        <v>11.7</v>
       </c>
       <c r="C39" t="n">
-        <v>39</v>
+        <v>496</v>
       </c>
       <c r="D39" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="E39" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F39" t="n">
-        <v>0.127</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>44542.58333333334</v>
+        <v>44499.58333333334</v>
       </c>
       <c r="B40" t="n">
-        <v>4.100000000000001</v>
+        <v>12.1</v>
       </c>
       <c r="C40" t="n">
-        <v>72</v>
+        <v>463</v>
       </c>
       <c r="D40" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="E40" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F40" t="n">
-        <v>0.001923076923076923</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>44542.625</v>
+        <v>44499.625</v>
       </c>
       <c r="B41" t="n">
-        <v>3.7</v>
+        <v>12</v>
       </c>
       <c r="C41" t="n">
-        <v>71</v>
+        <v>379</v>
       </c>
       <c r="D41" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="E41" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F41" t="n">
-        <v>0.4233333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>44542.66666666666</v>
+        <v>44499.66666666666</v>
       </c>
       <c r="B42" t="n">
-        <v>3</v>
+        <v>11.2</v>
       </c>
       <c r="C42" t="n">
-        <v>6</v>
+        <v>253</v>
       </c>
       <c r="D42" t="n">
-        <v>1</v>
-      </c>
-      <c r="E42" t="inlineStr"/>
+        <v>0.9</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F42" t="n">
-        <v>0.002083333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>44542.70833333334</v>
+        <v>44499.70833333334</v>
       </c>
       <c r="B43" t="n">
-        <v>2.6</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="D43" t="n">
-        <v>1</v>
-      </c>
-      <c r="E43" t="inlineStr"/>
+        <v>0.8</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F43" t="n">
-        <v>0.8255</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>44542.75</v>
+        <v>44499.75</v>
       </c>
       <c r="B44" t="n">
-        <v>2.3</v>
+        <v>6</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
@@ -2348,35 +2516,43 @@
       <c r="D44" t="n">
         <v>0.9</v>
       </c>
-      <c r="E44" t="inlineStr"/>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F44" t="n">
-        <v>0.003846153846153846</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>44542.79166666666</v>
+        <v>44499.79166666666</v>
       </c>
       <c r="B45" t="n">
-        <v>1.9</v>
+        <v>5.5</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="E45" t="inlineStr"/>
+        <v>0.9</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F45" t="n">
-        <v>0.001923076923076923</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>44542.83333333334</v>
+        <v>44499.83333333334</v>
       </c>
       <c r="B46" t="n">
-        <v>1.6</v>
+        <v>5</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
@@ -2384,17 +2560,21 @@
       <c r="D46" t="n">
         <v>0.8</v>
       </c>
-      <c r="E46" t="inlineStr"/>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F46" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>44542.875</v>
+        <v>44499.875</v>
       </c>
       <c r="B47" t="n">
-        <v>1.7</v>
+        <v>4.5</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
@@ -2402,45 +2582,57 @@
       <c r="D47" t="n">
         <v>0.8</v>
       </c>
-      <c r="E47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F47" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>44542.91666666666</v>
+        <v>44499.91666666666</v>
       </c>
       <c r="B48" t="n">
-        <v>2</v>
+        <v>4.4</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>0.7000000000000001</v>
-      </c>
-      <c r="E48" t="inlineStr"/>
+        <v>0.8</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F48" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>44542.95833333334</v>
+        <v>44499.95833333334</v>
       </c>
       <c r="B49" t="n">
-        <v>2.1</v>
+        <v>4.5</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="E49" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
       <c r="F49" t="n">
-        <v>0.1411111111111111</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2490,7 +2682,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Percipitation_mm</t>
+          <t>Precipitation_mm</t>
         </is>
       </c>
     </row>
@@ -2509,7 +2701,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -2531,7 +2723,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -2553,7 +2745,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -2575,7 +2767,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -2597,7 +2789,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -2619,7 +2811,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -2641,7 +2833,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -2663,7 +2855,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -2685,7 +2877,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -2707,7 +2899,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -2729,7 +2921,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -2751,7 +2943,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -2773,7 +2965,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -2795,7 +2987,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -2817,7 +3009,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -2839,7 +3031,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -2861,7 +3053,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -2883,7 +3075,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -2905,7 +3097,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -2927,7 +3119,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -2949,7 +3141,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -2971,7 +3163,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -2993,7 +3185,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -3015,7 +3207,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -3037,7 +3229,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -3059,7 +3251,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -3081,7 +3273,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -3103,7 +3295,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -3125,7 +3317,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -3147,7 +3339,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -3169,7 +3361,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -3191,7 +3383,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -3213,7 +3405,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -3235,7 +3427,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -3257,7 +3449,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -3279,7 +3471,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -3301,7 +3493,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -3323,7 +3515,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -3345,7 +3537,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -3367,7 +3559,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -3389,7 +3581,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -3411,7 +3603,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -3433,7 +3625,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -3455,7 +3647,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -3477,7 +3669,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -3499,7 +3691,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -3521,7 +3713,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -3543,7 +3735,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -3597,7 +3789,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Percipitation_mm</t>
+          <t>Precipitation_mm</t>
         </is>
       </c>
     </row>
@@ -3616,7 +3808,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -3638,7 +3830,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -3660,7 +3852,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -3682,7 +3874,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -3704,7 +3896,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -3726,7 +3918,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -3748,7 +3940,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -3770,7 +3962,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -3792,7 +3984,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -3814,7 +4006,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -3836,7 +4028,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -3858,7 +4050,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -3880,7 +4072,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -3902,7 +4094,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -3924,7 +4116,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -3946,7 +4138,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -3968,7 +4160,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -3990,7 +4182,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -4012,7 +4204,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -4034,7 +4226,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -4056,7 +4248,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -4078,7 +4270,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -4100,7 +4292,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -4122,7 +4314,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -4144,7 +4336,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -4166,7 +4358,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -4188,7 +4380,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -4210,7 +4402,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -4232,7 +4424,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -4254,7 +4446,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -4276,7 +4468,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -4298,7 +4490,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -4320,7 +4512,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -4342,7 +4534,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -4364,7 +4556,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -4386,7 +4578,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -4408,7 +4600,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -4430,7 +4622,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -4452,7 +4644,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -4474,7 +4666,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -4496,7 +4688,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -4518,7 +4710,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -4540,7 +4732,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -4562,7 +4754,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -4584,7 +4776,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -4606,7 +4798,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -4628,7 +4820,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -4650,7 +4842,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>fall</t>
         </is>
       </c>
       <c r="F49" t="n">

</xml_diff>